<commit_message>
App Semantica 1 stable - Checar sem 1 param
</commit_message>
<xml_diff>
--- a/Compiler/build/classes/res/Matrix_Sintactico.xlsx
+++ b/Compiler/build/classes/res/Matrix_Sintactico.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8280"/>
+    <workbookView windowWidth="21505" windowHeight="9051"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,10 +451,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="#,000_);[Red]\(#,000\)"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -521,64 +521,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,7 +538,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -607,8 +582,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -616,7 +608,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -636,16 +643,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,7 +690,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,7 +702,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,13 +738,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,121 +846,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,6 +857,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -879,16 +894,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -942,168 +957,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1171,54 +1171,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="60% - Énfasis6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Énfasis6" xfId="2" builtinId="51"/>
+    <cellStyle name="40% - Énfasis5" xfId="3" builtinId="47"/>
+    <cellStyle name="20% - Énfasis5" xfId="4" builtinId="46"/>
+    <cellStyle name="Énfasis5" xfId="5" builtinId="45"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
+    <cellStyle name="40% - Énfasis4" xfId="7" builtinId="43"/>
+    <cellStyle name="Moneda [0]" xfId="8" builtinId="7"/>
+    <cellStyle name="20% - Énfasis4" xfId="9" builtinId="42"/>
+    <cellStyle name="Énfasis4" xfId="10" builtinId="41"/>
+    <cellStyle name="20% - Énfasis3" xfId="11" builtinId="38"/>
+    <cellStyle name="Énfasis3" xfId="12" builtinId="37"/>
+    <cellStyle name="20% - Énfasis2" xfId="13" builtinId="34"/>
+    <cellStyle name="20% - Énfasis1" xfId="14" builtinId="30"/>
+    <cellStyle name="60% - Énfasis4" xfId="15" builtinId="44"/>
+    <cellStyle name="Énfasis1" xfId="16" builtinId="29"/>
+    <cellStyle name="Énfasis6" xfId="17" builtinId="49"/>
+    <cellStyle name="40% - Énfasis1" xfId="18" builtinId="31"/>
+    <cellStyle name="Incorrecto" xfId="19" builtinId="27"/>
+    <cellStyle name="60% - Énfasis5" xfId="20" builtinId="48"/>
+    <cellStyle name="Énfasis2" xfId="21" builtinId="33"/>
+    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
+    <cellStyle name="Total" xfId="23" builtinId="25"/>
+    <cellStyle name="Celda vinculada" xfId="24" builtinId="24"/>
+    <cellStyle name="Moneda" xfId="25" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="26" builtinId="5"/>
+    <cellStyle name="Texto explicativo" xfId="27" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="28" builtinId="16"/>
+    <cellStyle name="Celda de comprobación" xfId="29" builtinId="23"/>
+    <cellStyle name="Cálculo" xfId="30" builtinId="22"/>
+    <cellStyle name="60% - Énfasis3" xfId="31" builtinId="40"/>
+    <cellStyle name="Título 4" xfId="32" builtinId="19"/>
+    <cellStyle name="60% - Énfasis2" xfId="33" builtinId="36"/>
+    <cellStyle name="Título 3" xfId="34" builtinId="18"/>
+    <cellStyle name="60% - Énfasis1" xfId="35" builtinId="32"/>
+    <cellStyle name="Título 2" xfId="36" builtinId="17"/>
+    <cellStyle name="Neutro" xfId="37" builtinId="28"/>
+    <cellStyle name="Título" xfId="38" builtinId="15"/>
+    <cellStyle name="Salida" xfId="39" builtinId="21"/>
+    <cellStyle name="Coma" xfId="40" builtinId="3"/>
+    <cellStyle name="40% - Énfasis3" xfId="41" builtinId="39"/>
+    <cellStyle name="Entrada" xfId="42" builtinId="20"/>
+    <cellStyle name="Nota" xfId="43" builtinId="10"/>
+    <cellStyle name="Coma [0]" xfId="44" builtinId="6"/>
+    <cellStyle name="Hipervínculo visitado" xfId="45" builtinId="9"/>
+    <cellStyle name="40% - Énfasis2" xfId="46" builtinId="35"/>
+    <cellStyle name="20% - Énfasis6" xfId="47" builtinId="50"/>
+    <cellStyle name="Texto de advertencia" xfId="48" builtinId="11"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1489,28 +1489,28 @@
   <sheetPr/>
   <dimension ref="A1:DW127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="BP1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="U39" sqref="U39"/>
+      <selection pane="bottomLeft" activeCell="CE10" sqref="CE10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="3" max="3" width="10.8333333333333" customWidth="1"/>
-    <col min="4" max="4" width="10.975" customWidth="1"/>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
-    <col min="6" max="6" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="17.125" customWidth="1"/>
-    <col min="8" max="8" width="17.25" customWidth="1"/>
-    <col min="10" max="10" width="11.9416666666667" customWidth="1"/>
-    <col min="11" max="11" width="13.125" customWidth="1"/>
-    <col min="94" max="94" width="10.5" customWidth="1"/>
-    <col min="99" max="99" width="14.4416666666667" customWidth="1"/>
+    <col min="1" max="1" width="20.1259842519685" customWidth="1"/>
+    <col min="3" max="3" width="10.8346456692913" customWidth="1"/>
+    <col min="4" max="4" width="10.9763779527559" customWidth="1"/>
+    <col min="5" max="5" width="18.251968503937" customWidth="1"/>
+    <col min="6" max="6" width="15.748031496063" customWidth="1"/>
+    <col min="7" max="7" width="17.1259842519685" customWidth="1"/>
+    <col min="8" max="8" width="17.251968503937" customWidth="1"/>
+    <col min="10" max="10" width="11.9448818897638" customWidth="1"/>
+    <col min="11" max="11" width="13.1259842519685" customWidth="1"/>
+    <col min="94" max="94" width="10.503937007874" customWidth="1"/>
+    <col min="99" max="99" width="14.4409448818898" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:127">
+    <row r="1" ht="14.2" spans="1:127">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1829,7 +1829,7 @@
       <c r="DV1" s="17"/>
       <c r="DW1" s="17"/>
     </row>
-    <row r="2" ht="15" spans="1:127">
+    <row r="2" ht="14.2" spans="1:127">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="DV2" s="17"/>
       <c r="DW2" s="17"/>
     </row>
-    <row r="3" ht="15" spans="1:127">
+    <row r="3" ht="14.2" spans="1:127">
       <c r="A3" s="7" t="s">
         <v>94</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="DV3" s="17"/>
       <c r="DW3" s="17"/>
     </row>
-    <row r="4" ht="15" spans="1:127">
+    <row r="4" ht="14.2" spans="1:127">
       <c r="A4" s="7" t="s">
         <v>95</v>
       </c>
@@ -2797,7 +2797,7 @@
       <c r="DV4" s="17"/>
       <c r="DW4" s="17"/>
     </row>
-    <row r="5" ht="15" spans="1:127">
+    <row r="5" ht="14.2" spans="1:127">
       <c r="A5" s="7" t="s">
         <v>96</v>
       </c>
@@ -3120,7 +3120,7 @@
       <c r="DV5" s="17"/>
       <c r="DW5" s="17"/>
     </row>
-    <row r="6" ht="15" spans="1:127">
+    <row r="6" ht="14.2" spans="1:127">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="DV6" s="17"/>
       <c r="DW6" s="17"/>
     </row>
-    <row r="7" ht="15" spans="1:127">
+    <row r="7" ht="14.2" spans="1:127">
       <c r="A7" s="3" t="s">
         <v>98</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="DV7" s="17"/>
       <c r="DW7" s="17"/>
     </row>
-    <row r="8" ht="15" spans="1:127">
+    <row r="8" ht="14.2" spans="1:127">
       <c r="A8" s="3" t="s">
         <v>99</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="DV8" s="17"/>
       <c r="DW8" s="17"/>
     </row>
-    <row r="9" ht="15" spans="1:127">
+    <row r="9" ht="14.2" spans="1:127">
       <c r="A9" s="7" t="s">
         <v>100</v>
       </c>
@@ -4412,15 +4412,15 @@
       <c r="DV9" s="17"/>
       <c r="DW9" s="17"/>
     </row>
-    <row r="10" ht="15" spans="1:127">
+    <row r="10" ht="14.2" spans="1:127">
       <c r="A10" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="5">
         <v>608</v>
       </c>
-      <c r="C10" s="5">
-        <v>608</v>
+      <c r="C10" s="4">
+        <v>26</v>
       </c>
       <c r="D10" s="5">
         <v>608</v>
@@ -4735,7 +4735,7 @@
       <c r="DV10" s="17"/>
       <c r="DW10" s="17"/>
     </row>
-    <row r="11" ht="15" spans="1:127">
+    <row r="11" ht="14.2" spans="1:127">
       <c r="A11" s="7" t="s">
         <v>102</v>
       </c>
@@ -5058,7 +5058,7 @@
       <c r="DV11" s="17"/>
       <c r="DW11" s="17"/>
     </row>
-    <row r="12" ht="15" spans="1:127">
+    <row r="12" ht="14.2" spans="1:127">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
@@ -5381,7 +5381,7 @@
       <c r="DV12" s="17"/>
       <c r="DW12" s="17"/>
     </row>
-    <row r="13" ht="15" spans="1:127">
+    <row r="13" ht="14.2" spans="1:127">
       <c r="A13" s="7" t="s">
         <v>104</v>
       </c>
@@ -5704,7 +5704,7 @@
       <c r="DV13" s="17"/>
       <c r="DW13" s="17"/>
     </row>
-    <row r="14" ht="15" spans="1:127">
+    <row r="14" ht="14.2" spans="1:127">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
@@ -6027,7 +6027,7 @@
       <c r="DV14" s="17"/>
       <c r="DW14" s="17"/>
     </row>
-    <row r="15" ht="15" spans="1:127">
+    <row r="15" ht="14.2" spans="1:127">
       <c r="A15" s="7" t="s">
         <v>106</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="DV15" s="17"/>
       <c r="DW15" s="17"/>
     </row>
-    <row r="16" ht="15" spans="1:127">
+    <row r="16" ht="14.2" spans="1:127">
       <c r="A16" s="3" t="s">
         <v>107</v>
       </c>
@@ -6673,7 +6673,7 @@
       <c r="DV16" s="17"/>
       <c r="DW16" s="17"/>
     </row>
-    <row r="17" ht="15" spans="1:127">
+    <row r="17" ht="14.2" spans="1:127">
       <c r="A17" s="7" t="s">
         <v>108</v>
       </c>
@@ -6996,7 +6996,7 @@
       <c r="DV17" s="17"/>
       <c r="DW17" s="17"/>
     </row>
-    <row r="18" ht="15" spans="1:127">
+    <row r="18" ht="14.2" spans="1:127">
       <c r="A18" s="3" t="s">
         <v>109</v>
       </c>
@@ -7319,7 +7319,7 @@
       <c r="DV18" s="17"/>
       <c r="DW18" s="17"/>
     </row>
-    <row r="19" ht="15" spans="1:127">
+    <row r="19" ht="14.2" spans="1:127">
       <c r="A19" s="7" t="s">
         <v>110</v>
       </c>
@@ -7642,7 +7642,7 @@
       <c r="DV19" s="17"/>
       <c r="DW19" s="17"/>
     </row>
-    <row r="20" ht="15" spans="1:127">
+    <row r="20" ht="14.2" spans="1:127">
       <c r="A20" s="7" t="s">
         <v>111</v>
       </c>
@@ -7965,7 +7965,7 @@
       <c r="DV20" s="17"/>
       <c r="DW20" s="17"/>
     </row>
-    <row r="21" ht="15" spans="1:127">
+    <row r="21" ht="14.2" spans="1:127">
       <c r="A21" s="7" t="s">
         <v>112</v>
       </c>
@@ -8288,7 +8288,7 @@
       <c r="DV21" s="17"/>
       <c r="DW21" s="17"/>
     </row>
-    <row r="22" ht="15" spans="1:127">
+    <row r="22" ht="14.2" spans="1:127">
       <c r="A22" s="7" t="s">
         <v>113</v>
       </c>
@@ -8611,7 +8611,7 @@
       <c r="DV22" s="17"/>
       <c r="DW22" s="17"/>
     </row>
-    <row r="23" ht="15" spans="1:127">
+    <row r="23" ht="14.2" spans="1:127">
       <c r="A23" s="3" t="s">
         <v>114</v>
       </c>
@@ -8934,7 +8934,7 @@
       <c r="DV23" s="17"/>
       <c r="DW23" s="17"/>
     </row>
-    <row r="24" ht="15" spans="1:127">
+    <row r="24" ht="14.2" spans="1:127">
       <c r="A24" s="7" t="s">
         <v>115</v>
       </c>
@@ -9257,7 +9257,7 @@
       <c r="DV24" s="17"/>
       <c r="DW24" s="17"/>
     </row>
-    <row r="25" ht="15" spans="1:127">
+    <row r="25" ht="14.2" spans="1:127">
       <c r="A25" s="3" t="s">
         <v>116</v>
       </c>
@@ -9580,7 +9580,7 @@
       <c r="DV25" s="17"/>
       <c r="DW25" s="17"/>
     </row>
-    <row r="26" ht="15" spans="1:127">
+    <row r="26" ht="14.2" spans="1:127">
       <c r="A26" s="7" t="s">
         <v>117</v>
       </c>
@@ -9903,7 +9903,7 @@
       <c r="DV26" s="17"/>
       <c r="DW26" s="17"/>
     </row>
-    <row r="27" ht="15" spans="1:127">
+    <row r="27" ht="14.2" spans="1:127">
       <c r="A27" s="3" t="s">
         <v>118</v>
       </c>
@@ -10226,7 +10226,7 @@
       <c r="DV27" s="17"/>
       <c r="DW27" s="17"/>
     </row>
-    <row r="28" ht="15" spans="1:127">
+    <row r="28" ht="14.2" spans="1:127">
       <c r="A28" s="7" t="s">
         <v>119</v>
       </c>
@@ -10549,7 +10549,7 @@
       <c r="DV28" s="17"/>
       <c r="DW28" s="17"/>
     </row>
-    <row r="29" ht="15" spans="1:127">
+    <row r="29" ht="14.2" spans="1:127">
       <c r="A29" s="3" t="s">
         <v>120</v>
       </c>
@@ -10872,7 +10872,7 @@
       <c r="DV29" s="17"/>
       <c r="DW29" s="17"/>
     </row>
-    <row r="30" ht="15" spans="1:127">
+    <row r="30" ht="14.2" spans="1:127">
       <c r="A30" s="7" t="s">
         <v>121</v>
       </c>
@@ -11195,7 +11195,7 @@
       <c r="DV30" s="17"/>
       <c r="DW30" s="17"/>
     </row>
-    <row r="31" ht="15" spans="1:127">
+    <row r="31" ht="14.2" spans="1:127">
       <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
@@ -11518,7 +11518,7 @@
       <c r="DV31" s="17"/>
       <c r="DW31" s="17"/>
     </row>
-    <row r="32" ht="15" spans="1:127">
+    <row r="32" ht="14.2" spans="1:127">
       <c r="A32" s="7" t="s">
         <v>123</v>
       </c>
@@ -11841,7 +11841,7 @@
       <c r="DV32" s="17"/>
       <c r="DW32" s="17"/>
     </row>
-    <row r="33" ht="15" spans="1:127">
+    <row r="33" ht="14.2" spans="1:127">
       <c r="A33" s="3" t="s">
         <v>124</v>
       </c>
@@ -12164,7 +12164,7 @@
       <c r="DV33" s="17"/>
       <c r="DW33" s="17"/>
     </row>
-    <row r="34" ht="15" spans="1:127">
+    <row r="34" ht="14.2" spans="1:127">
       <c r="A34" s="7" t="s">
         <v>125</v>
       </c>
@@ -12487,7 +12487,7 @@
       <c r="DV34" s="17"/>
       <c r="DW34" s="17"/>
     </row>
-    <row r="35" ht="15" spans="1:127">
+    <row r="35" ht="14.2" spans="1:127">
       <c r="A35" s="3" t="s">
         <v>126</v>
       </c>
@@ -12810,7 +12810,7 @@
       <c r="DV35" s="17"/>
       <c r="DW35" s="17"/>
     </row>
-    <row r="36" ht="15" spans="1:127">
+    <row r="36" ht="14.2" spans="1:127">
       <c r="A36" s="7" t="s">
         <v>127</v>
       </c>
@@ -13133,7 +13133,7 @@
       <c r="DV36" s="17"/>
       <c r="DW36" s="17"/>
     </row>
-    <row r="37" ht="15" spans="1:127">
+    <row r="37" ht="14.2" spans="1:127">
       <c r="A37" s="3" t="s">
         <v>128</v>
       </c>
@@ -13456,7 +13456,7 @@
       <c r="DV37" s="17"/>
       <c r="DW37" s="17"/>
     </row>
-    <row r="38" ht="15" spans="1:127">
+    <row r="38" ht="14.2" spans="1:127">
       <c r="A38" s="7" t="s">
         <v>129</v>
       </c>
@@ -13779,7 +13779,7 @@
       <c r="DV38" s="17"/>
       <c r="DW38" s="17"/>
     </row>
-    <row r="39" ht="15" spans="1:127">
+    <row r="39" ht="14.2" spans="1:127">
       <c r="A39" s="7" t="s">
         <v>130</v>
       </c>
@@ -14102,7 +14102,7 @@
       <c r="DV39" s="17"/>
       <c r="DW39" s="17"/>
     </row>
-    <row r="40" ht="15" spans="1:127">
+    <row r="40" ht="14.2" spans="1:127">
       <c r="A40" s="7" t="s">
         <v>131</v>
       </c>
@@ -14425,7 +14425,7 @@
       <c r="DV40" s="17"/>
       <c r="DW40" s="17"/>
     </row>
-    <row r="41" ht="15" spans="1:127">
+    <row r="41" ht="14.2" spans="1:127">
       <c r="A41" s="7" t="s">
         <v>132</v>
       </c>
@@ -14748,7 +14748,7 @@
       <c r="DV41" s="17"/>
       <c r="DW41" s="17"/>
     </row>
-    <row r="42" ht="15" spans="1:127">
+    <row r="42" ht="14.2" spans="1:127">
       <c r="A42" s="3" t="s">
         <v>133</v>
       </c>
@@ -15071,7 +15071,7 @@
       <c r="DV42" s="17"/>
       <c r="DW42" s="17"/>
     </row>
-    <row r="43" ht="15" spans="1:127">
+    <row r="43" ht="14.2" spans="1:127">
       <c r="A43" s="3" t="s">
         <v>134</v>
       </c>
@@ -15394,7 +15394,7 @@
       <c r="DV43" s="17"/>
       <c r="DW43" s="17"/>
     </row>
-    <row r="44" ht="15" spans="1:127">
+    <row r="44" ht="14.2" spans="1:127">
       <c r="A44" s="3" t="s">
         <v>135</v>
       </c>
@@ -15717,7 +15717,7 @@
       <c r="DV44" s="17"/>
       <c r="DW44" s="17"/>
     </row>
-    <row r="45" ht="15" spans="1:127">
+    <row r="45" ht="14.2" spans="1:127">
       <c r="A45" s="7" t="s">
         <v>136</v>
       </c>
@@ -16040,7 +16040,7 @@
       <c r="DV45" s="17"/>
       <c r="DW45" s="17"/>
     </row>
-    <row r="46" ht="15" spans="1:127">
+    <row r="46" ht="14.2" spans="1:127">
       <c r="A46" s="7" t="s">
         <v>137</v>
       </c>
@@ -16363,7 +16363,7 @@
       <c r="DV46" s="17"/>
       <c r="DW46" s="17"/>
     </row>
-    <row r="47" ht="15" spans="1:127">
+    <row r="47" ht="14.2" spans="1:127">
       <c r="A47" s="7" t="s">
         <v>138</v>
       </c>
@@ -16686,7 +16686,7 @@
       <c r="DV47" s="17"/>
       <c r="DW47" s="17"/>
     </row>
-    <row r="48" ht="15" spans="1:127">
+    <row r="48" ht="14.2" spans="1:127">
       <c r="A48" s="3" t="s">
         <v>139</v>
       </c>
@@ -17009,7 +17009,7 @@
       <c r="DV48" s="17"/>
       <c r="DW48" s="17"/>
     </row>
-    <row r="49" ht="15" spans="1:127">
+    <row r="49" ht="14.2" spans="1:127">
       <c r="A49" s="7" t="s">
         <v>140</v>
       </c>
@@ -17332,7 +17332,7 @@
       <c r="DV49" s="17"/>
       <c r="DW49" s="17"/>
     </row>
-    <row r="50" ht="15" spans="1:127">
+    <row r="50" ht="14.2" spans="1:127">
       <c r="A50" s="3" t="s">
         <v>141</v>
       </c>
@@ -17655,7 +17655,7 @@
       <c r="DV50" s="17"/>
       <c r="DW50" s="17"/>
     </row>
-    <row r="51" ht="15" spans="1:127">
+    <row r="51" ht="14.2" spans="1:127">
       <c r="A51" s="9" t="s">
         <v>142</v>
       </c>
@@ -17978,7 +17978,7 @@
       <c r="DV51" s="17"/>
       <c r="DW51" s="17"/>
     </row>
-    <row r="52" ht="15" spans="1:127">
+    <row r="52" ht="14.2" spans="1:127">
       <c r="A52" s="10"/>
       <c r="B52" s="11">
         <v>0</v>
@@ -18389,7 +18389,7 @@
       <c r="DV52" s="17"/>
       <c r="DW52" s="17"/>
     </row>
-    <row r="53" ht="15" spans="1:127">
+    <row r="53" ht="14.2" spans="1:127">
       <c r="A53" s="12"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -18516,7 +18516,7 @@
       <c r="DV53" s="17"/>
       <c r="DW53" s="17"/>
     </row>
-    <row r="54" ht="15" spans="1:127">
+    <row r="54" ht="14.2" spans="1:127">
       <c r="A54" s="13"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -18643,7 +18643,7 @@
       <c r="DV54" s="17"/>
       <c r="DW54" s="17"/>
     </row>
-    <row r="55" ht="15" spans="1:127">
+    <row r="55" ht="14.2" spans="1:127">
       <c r="A55" s="13"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -18770,7 +18770,7 @@
       <c r="DV55" s="17"/>
       <c r="DW55" s="17"/>
     </row>
-    <row r="56" ht="15" spans="1:127">
+    <row r="56" ht="14.2" spans="1:127">
       <c r="A56" s="13"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -18897,7 +18897,7 @@
       <c r="DV56" s="17"/>
       <c r="DW56" s="17"/>
     </row>
-    <row r="57" ht="15" spans="1:127">
+    <row r="57" ht="14.2" spans="1:127">
       <c r="A57" s="13"/>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -19024,7 +19024,7 @@
       <c r="DV57" s="17"/>
       <c r="DW57" s="17"/>
     </row>
-    <row r="58" ht="15" spans="1:127">
+    <row r="58" ht="14.2" spans="1:127">
       <c r="A58" s="13"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -19151,7 +19151,7 @@
       <c r="DV58" s="17"/>
       <c r="DW58" s="17"/>
     </row>
-    <row r="59" ht="15" spans="1:127">
+    <row r="59" ht="14.2" spans="1:127">
       <c r="A59" s="10"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -19278,7 +19278,7 @@
       <c r="DV59" s="17"/>
       <c r="DW59" s="17"/>
     </row>
-    <row r="60" ht="15" spans="1:127">
+    <row r="60" ht="14.2" spans="1:127">
       <c r="A60" s="13"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -19405,7 +19405,7 @@
       <c r="DV60" s="17"/>
       <c r="DW60" s="17"/>
     </row>
-    <row r="61" ht="15" spans="1:127">
+    <row r="61" ht="14.2" spans="1:127">
       <c r="A61" s="13"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -19532,7 +19532,7 @@
       <c r="DV61" s="17"/>
       <c r="DW61" s="17"/>
     </row>
-    <row r="62" ht="15" spans="1:127">
+    <row r="62" ht="14.2" spans="1:127">
       <c r="A62" s="13"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -19659,7 +19659,7 @@
       <c r="DV62" s="17"/>
       <c r="DW62" s="17"/>
     </row>
-    <row r="63" ht="15" spans="1:127">
+    <row r="63" ht="14.2" spans="1:127">
       <c r="A63" s="13"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -19786,7 +19786,7 @@
       <c r="DV63" s="17"/>
       <c r="DW63" s="17"/>
     </row>
-    <row r="64" ht="15" spans="1:127">
+    <row r="64" ht="14.2" spans="1:127">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -19913,7 +19913,7 @@
       <c r="DV64" s="17"/>
       <c r="DW64" s="17"/>
     </row>
-    <row r="65" ht="15" spans="1:127">
+    <row r="65" ht="14.2" spans="1:127">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -20040,7 +20040,7 @@
       <c r="DV65" s="17"/>
       <c r="DW65" s="17"/>
     </row>
-    <row r="66" ht="15" spans="1:127">
+    <row r="66" ht="14.2" spans="1:127">
       <c r="A66" s="13"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -20167,7 +20167,7 @@
       <c r="DV66" s="17"/>
       <c r="DW66" s="17"/>
     </row>
-    <row r="67" ht="15" spans="1:127">
+    <row r="67" ht="14.2" spans="1:127">
       <c r="A67" s="13"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -20294,7 +20294,7 @@
       <c r="DV67" s="17"/>
       <c r="DW67" s="17"/>
     </row>
-    <row r="68" ht="15" spans="1:127">
+    <row r="68" ht="14.2" spans="1:127">
       <c r="A68" s="13"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -20421,7 +20421,7 @@
       <c r="DV68" s="17"/>
       <c r="DW68" s="17"/>
     </row>
-    <row r="69" ht="15" spans="1:127">
+    <row r="69" ht="14.2" spans="1:127">
       <c r="A69" s="13"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -20548,7 +20548,7 @@
       <c r="DV69" s="17"/>
       <c r="DW69" s="17"/>
     </row>
-    <row r="70" ht="15" spans="1:127">
+    <row r="70" ht="14.2" spans="1:127">
       <c r="A70" s="13"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -20675,7 +20675,7 @@
       <c r="DV70" s="17"/>
       <c r="DW70" s="17"/>
     </row>
-    <row r="71" ht="15" spans="1:127">
+    <row r="71" ht="14.2" spans="1:127">
       <c r="A71" s="13"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
@@ -20802,7 +20802,7 @@
       <c r="DV71" s="17"/>
       <c r="DW71" s="17"/>
     </row>
-    <row r="72" ht="15" spans="1:127">
+    <row r="72" ht="14.2" spans="1:127">
       <c r="A72" s="13"/>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
@@ -20929,7 +20929,7 @@
       <c r="DV72" s="17"/>
       <c r="DW72" s="17"/>
     </row>
-    <row r="73" ht="15" spans="1:127">
+    <row r="73" ht="14.2" spans="1:127">
       <c r="A73" s="13"/>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -21056,7 +21056,7 @@
       <c r="DV73" s="17"/>
       <c r="DW73" s="17"/>
     </row>
-    <row r="74" ht="15" spans="1:127">
+    <row r="74" ht="14.2" spans="1:127">
       <c r="A74" s="13"/>
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
@@ -21183,7 +21183,7 @@
       <c r="DV74" s="17"/>
       <c r="DW74" s="17"/>
     </row>
-    <row r="75" ht="15" spans="1:127">
+    <row r="75" ht="14.2" spans="1:127">
       <c r="A75" s="13"/>
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
@@ -21310,7 +21310,7 @@
       <c r="DV75" s="17"/>
       <c r="DW75" s="17"/>
     </row>
-    <row r="76" ht="15" spans="1:127">
+    <row r="76" ht="14.2" spans="1:127">
       <c r="A76" s="13"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -21437,7 +21437,7 @@
       <c r="DV76" s="17"/>
       <c r="DW76" s="17"/>
     </row>
-    <row r="77" ht="15" spans="1:127">
+    <row r="77" ht="14.2" spans="1:127">
       <c r="A77" s="13"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -21564,7 +21564,7 @@
       <c r="DV77" s="17"/>
       <c r="DW77" s="17"/>
     </row>
-    <row r="78" ht="15" spans="1:127">
+    <row r="78" ht="14.2" spans="1:127">
       <c r="A78" s="13"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -21691,7 +21691,7 @@
       <c r="DV78" s="17"/>
       <c r="DW78" s="17"/>
     </row>
-    <row r="79" ht="15" spans="1:127">
+    <row r="79" ht="14.2" spans="1:127">
       <c r="A79" s="13"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -21818,7 +21818,7 @@
       <c r="DV79" s="17"/>
       <c r="DW79" s="17"/>
     </row>
-    <row r="80" ht="15" spans="1:127">
+    <row r="80" ht="14.2" spans="1:127">
       <c r="A80" s="13"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -21945,7 +21945,7 @@
       <c r="DV80" s="17"/>
       <c r="DW80" s="17"/>
     </row>
-    <row r="81" ht="15" spans="1:127">
+    <row r="81" ht="14.2" spans="1:127">
       <c r="A81" s="13"/>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -22072,7 +22072,7 @@
       <c r="DV81" s="17"/>
       <c r="DW81" s="17"/>
     </row>
-    <row r="82" ht="15" spans="1:127">
+    <row r="82" ht="14.2" spans="1:127">
       <c r="A82" s="13"/>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -22199,7 +22199,7 @@
       <c r="DV82" s="17"/>
       <c r="DW82" s="17"/>
     </row>
-    <row r="83" ht="15" spans="1:127">
+    <row r="83" ht="14.2" spans="1:127">
       <c r="A83" s="13"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -22326,7 +22326,7 @@
       <c r="DV83" s="17"/>
       <c r="DW83" s="17"/>
     </row>
-    <row r="84" ht="15" spans="1:127">
+    <row r="84" ht="14.2" spans="1:127">
       <c r="A84" s="13"/>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
@@ -22453,7 +22453,7 @@
       <c r="DV84" s="17"/>
       <c r="DW84" s="17"/>
     </row>
-    <row r="85" ht="15" spans="1:127">
+    <row r="85" ht="14.2" spans="1:127">
       <c r="A85" s="13"/>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
@@ -22580,7 +22580,7 @@
       <c r="DV85" s="17"/>
       <c r="DW85" s="17"/>
     </row>
-    <row r="86" ht="15" spans="1:127">
+    <row r="86" ht="14.2" spans="1:127">
       <c r="A86" s="13"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
@@ -22707,7 +22707,7 @@
       <c r="DV86" s="17"/>
       <c r="DW86" s="17"/>
     </row>
-    <row r="87" ht="15" spans="1:127">
+    <row r="87" ht="14.2" spans="1:127">
       <c r="A87" s="13"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
@@ -22834,7 +22834,7 @@
       <c r="DV87" s="17"/>
       <c r="DW87" s="17"/>
     </row>
-    <row r="88" ht="15" spans="1:127">
+    <row r="88" ht="14.2" spans="1:127">
       <c r="A88" s="13"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
@@ -22961,7 +22961,7 @@
       <c r="DV88" s="17"/>
       <c r="DW88" s="17"/>
     </row>
-    <row r="89" ht="15" spans="1:127">
+    <row r="89" ht="14.2" spans="1:127">
       <c r="A89" s="13"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -23088,7 +23088,7 @@
       <c r="DV89" s="17"/>
       <c r="DW89" s="17"/>
     </row>
-    <row r="90" ht="15" spans="1:127">
+    <row r="90" ht="14.2" spans="1:127">
       <c r="A90" s="13"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -23215,7 +23215,7 @@
       <c r="DV90" s="17"/>
       <c r="DW90" s="17"/>
     </row>
-    <row r="91" ht="15" spans="1:127">
+    <row r="91" ht="14.2" spans="1:127">
       <c r="A91" s="13"/>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -23342,7 +23342,7 @@
       <c r="DV91" s="17"/>
       <c r="DW91" s="17"/>
     </row>
-    <row r="92" ht="15" spans="1:127">
+    <row r="92" ht="14.2" spans="1:127">
       <c r="A92" s="18"/>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -23427,7 +23427,7 @@
       <c r="DV92" s="17"/>
       <c r="DW92" s="17"/>
     </row>
-    <row r="93" ht="15" spans="1:127">
+    <row r="93" ht="14.2" spans="1:127">
       <c r="A93" s="18"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -23512,7 +23512,7 @@
       <c r="DV93" s="17"/>
       <c r="DW93" s="17"/>
     </row>
-    <row r="94" ht="15" spans="1:127">
+    <row r="94" ht="14.2" spans="1:127">
       <c r="A94" s="18"/>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
@@ -23597,7 +23597,7 @@
       <c r="DV94" s="17"/>
       <c r="DW94" s="17"/>
     </row>
-    <row r="95" ht="15" spans="1:127">
+    <row r="95" ht="14.2" spans="1:127">
       <c r="A95" s="18"/>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
@@ -23682,7 +23682,7 @@
       <c r="DV95" s="17"/>
       <c r="DW95" s="17"/>
     </row>
-    <row r="96" ht="15" spans="1:127">
+    <row r="96" ht="14.2" spans="1:127">
       <c r="A96" s="18"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
@@ -23767,7 +23767,7 @@
       <c r="DV96" s="17"/>
       <c r="DW96" s="17"/>
     </row>
-    <row r="97" ht="15" spans="1:127">
+    <row r="97" ht="14.2" spans="1:127">
       <c r="A97" s="18"/>
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
@@ -23852,7 +23852,7 @@
       <c r="DV97" s="17"/>
       <c r="DW97" s="17"/>
     </row>
-    <row r="98" ht="15" spans="1:127">
+    <row r="98" ht="14.2" spans="1:127">
       <c r="A98" s="18"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -23937,7 +23937,7 @@
       <c r="DV98" s="17"/>
       <c r="DW98" s="17"/>
     </row>
-    <row r="99" ht="15" spans="2:127">
+    <row r="99" ht="14.2" spans="2:127">
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
@@ -24021,7 +24021,7 @@
       <c r="DV99" s="17"/>
       <c r="DW99" s="17"/>
     </row>
-    <row r="100" ht="15" spans="2:127">
+    <row r="100" ht="14.2" spans="2:127">
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
@@ -24105,7 +24105,7 @@
       <c r="DV100" s="17"/>
       <c r="DW100" s="17"/>
     </row>
-    <row r="101" ht="15" spans="2:127">
+    <row r="101" ht="14.2" spans="2:127">
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
@@ -24189,7 +24189,7 @@
       <c r="DV101" s="17"/>
       <c r="DW101" s="17"/>
     </row>
-    <row r="102" ht="15" spans="2:127">
+    <row r="102" ht="14.2" spans="2:127">
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
@@ -24273,7 +24273,7 @@
       <c r="DV102" s="17"/>
       <c r="DW102" s="17"/>
     </row>
-    <row r="103" ht="15" spans="2:127">
+    <row r="103" ht="14.2" spans="2:127">
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
@@ -24357,7 +24357,7 @@
       <c r="DV103" s="17"/>
       <c r="DW103" s="17"/>
     </row>
-    <row r="104" ht="15" spans="2:127">
+    <row r="104" ht="14.2" spans="2:127">
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
@@ -24441,7 +24441,7 @@
       <c r="DV104" s="17"/>
       <c r="DW104" s="17"/>
     </row>
-    <row r="105" ht="15" spans="2:127">
+    <row r="105" ht="14.2" spans="2:127">
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
@@ -24525,7 +24525,7 @@
       <c r="DV105" s="17"/>
       <c r="DW105" s="17"/>
     </row>
-    <row r="106" ht="15" spans="2:127">
+    <row r="106" ht="14.2" spans="2:127">
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -24609,7 +24609,7 @@
       <c r="DV106" s="17"/>
       <c r="DW106" s="17"/>
     </row>
-    <row r="107" ht="15" spans="2:127">
+    <row r="107" ht="14.2" spans="2:127">
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -24693,7 +24693,7 @@
       <c r="DV107" s="17"/>
       <c r="DW107" s="17"/>
     </row>
-    <row r="108" ht="15" spans="2:127">
+    <row r="108" ht="14.2" spans="2:127">
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -24777,7 +24777,7 @@
       <c r="DV108" s="17"/>
       <c r="DW108" s="17"/>
     </row>
-    <row r="109" ht="15" spans="2:127">
+    <row r="109" ht="14.2" spans="2:127">
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
@@ -24861,7 +24861,7 @@
       <c r="DV109" s="17"/>
       <c r="DW109" s="17"/>
     </row>
-    <row r="110" ht="15" spans="2:127">
+    <row r="110" ht="14.2" spans="2:127">
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -24945,7 +24945,7 @@
       <c r="DV110" s="17"/>
       <c r="DW110" s="17"/>
     </row>
-    <row r="111" ht="15" spans="2:127">
+    <row r="111" ht="14.2" spans="2:127">
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
@@ -25029,7 +25029,7 @@
       <c r="DV111" s="17"/>
       <c r="DW111" s="17"/>
     </row>
-    <row r="112" ht="15" spans="2:127">
+    <row r="112" ht="14.2" spans="2:127">
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
@@ -25113,7 +25113,7 @@
       <c r="DV112" s="17"/>
       <c r="DW112" s="17"/>
     </row>
-    <row r="113" ht="15" spans="2:127">
+    <row r="113" ht="14.2" spans="2:127">
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
@@ -25197,7 +25197,7 @@
       <c r="DV113" s="17"/>
       <c r="DW113" s="17"/>
     </row>
-    <row r="114" ht="15" spans="2:127">
+    <row r="114" ht="14.2" spans="2:127">
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
@@ -25281,7 +25281,7 @@
       <c r="DV114" s="17"/>
       <c r="DW114" s="17"/>
     </row>
-    <row r="115" ht="15" spans="2:127">
+    <row r="115" ht="14.2" spans="2:127">
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
@@ -25365,7 +25365,7 @@
       <c r="DV115" s="17"/>
       <c r="DW115" s="17"/>
     </row>
-    <row r="116" ht="15" spans="2:127">
+    <row r="116" ht="14.2" spans="2:127">
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -25449,7 +25449,7 @@
       <c r="DV116" s="17"/>
       <c r="DW116" s="17"/>
     </row>
-    <row r="117" ht="15" spans="2:127">
+    <row r="117" ht="14.2" spans="2:127">
       <c r="B117" s="11"/>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
@@ -25533,7 +25533,7 @@
       <c r="DV117" s="17"/>
       <c r="DW117" s="17"/>
     </row>
-    <row r="118" ht="15" spans="2:127">
+    <row r="118" ht="14.2" spans="2:127">
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
@@ -25617,7 +25617,7 @@
       <c r="DV118" s="17"/>
       <c r="DW118" s="17"/>
     </row>
-    <row r="119" ht="15" spans="2:127">
+    <row r="119" ht="14.2" spans="2:127">
       <c r="B119" s="11"/>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
@@ -25701,7 +25701,7 @@
       <c r="DV119" s="17"/>
       <c r="DW119" s="17"/>
     </row>
-    <row r="120" ht="15" spans="2:127">
+    <row r="120" ht="14.2" spans="2:127">
       <c r="B120" s="11"/>
       <c r="C120" s="11"/>
       <c r="D120" s="11"/>
@@ -25785,7 +25785,7 @@
       <c r="DV120" s="17"/>
       <c r="DW120" s="17"/>
     </row>
-    <row r="121" ht="15" spans="2:127">
+    <row r="121" ht="14.2" spans="2:127">
       <c r="B121" s="11"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
@@ -25869,7 +25869,7 @@
       <c r="DV121" s="17"/>
       <c r="DW121" s="17"/>
     </row>
-    <row r="122" ht="15" spans="2:127">
+    <row r="122" ht="14.2" spans="2:127">
       <c r="B122" s="11"/>
       <c r="C122" s="11"/>
       <c r="D122" s="11"/>
@@ -25953,7 +25953,7 @@
       <c r="DV122" s="17"/>
       <c r="DW122" s="17"/>
     </row>
-    <row r="123" ht="15" spans="2:99">
+    <row r="123" ht="14.2" spans="2:99">
       <c r="B123" s="11"/>
       <c r="C123" s="11"/>
       <c r="D123" s="11"/>
@@ -26009,13 +26009,13 @@
       <c r="BB123" s="11"/>
       <c r="CU123" s="11"/>
     </row>
-    <row r="124" ht="15" spans="99:99">
+    <row r="124" ht="14.2" spans="99:99">
       <c r="CU124" s="11"/>
     </row>
-    <row r="125" ht="15" spans="99:99">
+    <row r="125" ht="14.2" spans="99:99">
       <c r="CU125" s="11"/>
     </row>
-    <row r="127" ht="15" spans="99:99">
+    <row r="127" ht="14.2" spans="99:99">
       <c r="CU127" s="11"/>
     </row>
   </sheetData>

</xml_diff>